<commit_message>
Cambios a ser confirmados: 	modificado:     docs/Resultados.xlsx 	modificado:     docs/Word_list.xlsx 	modificado:     respaldo/Word_list.xlsx 	modificado:     test/funciones_test.py 	modificado:     vocabulario/classes.py
</commit_message>
<xml_diff>
--- a/docs/Resultados.xlsx
+++ b/docs/Resultados.xlsx
@@ -162,16 +162,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -395,6 +394,7 @@
         <v>68</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Ajuste de sintaxis de la clase Practice
</commit_message>
<xml_diff>
--- a/docs/Resultados.xlsx
+++ b/docs/Resultados.xlsx
@@ -162,15 +162,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1048576"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -371,30 +372,6 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="n">
-        <v>44358</v>
-      </c>
-      <c r="B22" s="0" t="n">
-        <v>68</v>
-      </c>
-      <c r="C22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" s="0" t="n">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>